<commit_message>
my changes on excel shhet
</commit_message>
<xml_diff>
--- a/Open Source task.xlsx
+++ b/Open Source task.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esraa Taher 2\Teaching\Open Source (credit 2024)\Open Source Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habiba said\Desktop\openn sourcee taskk\Security-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F655D791-30F8-43EC-9757-0AEF2D716D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4054F23-EF11-4ECC-9A60-90E1FAB71E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -45,16 +34,33 @@
   </si>
   <si>
     <t>Repo Link</t>
+  </si>
+  <si>
+    <t>habubasaid22@gmail.com</t>
+  </si>
+  <si>
+    <t>habibasaid22</t>
+  </si>
+  <si>
+    <t>https://github.com/Karim3bdelmn3m/our-project.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,14 +104,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,20 +447,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B88C28-23A0-4FB2-A45B-5BE272931FEB}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" customWidth="1"/>
+    <col min="2" max="2" width="17.69921875" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +471,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{117A6C6F-5CA2-4DA5-923C-DEF5C8DBCC19}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>